<commit_message>
update new assay data
</commit_message>
<xml_diff>
--- a/data/nano_bert_lineplot_braf.xlsx
+++ b/data/nano_bert_lineplot_braf.xlsx
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1062,10 +1062,10 @@
         <v>0.0257392301639433</v>
       </c>
       <c r="D2" s="2">
-        <v>1.02977653723633</v>
+        <v>0.982952696</v>
       </c>
       <c r="E2" s="2">
-        <v>0.0328703981775127</v>
+        <v>0.090851038</v>
       </c>
       <c r="F2">
         <v>1.0790400761768</v>
@@ -1085,10 +1085,10 @@
         <v>0.116087896916201</v>
       </c>
       <c r="D3" s="2">
-        <v>0.963293300670989</v>
+        <v>0.963293301</v>
       </c>
       <c r="E3" s="2">
-        <v>0.121493205103401</v>
+        <v>0.121493205</v>
       </c>
       <c r="F3">
         <v>1.11545277786692</v>
@@ -1108,10 +1108,10 @@
         <v>0.0572822550377937</v>
       </c>
       <c r="D4" s="2">
-        <v>1.00279450057724</v>
+        <v>1.002794501</v>
       </c>
       <c r="E4" s="2">
-        <v>0.07107138166196</v>
+        <v>0.071071382</v>
       </c>
       <c r="F4">
         <v>1.09929131894269</v>
@@ -1131,10 +1131,10 @@
         <v>0.161823528560927</v>
       </c>
       <c r="D5" s="2">
-        <v>0.969787650305422</v>
+        <v>0.96978765</v>
       </c>
       <c r="E5" s="2">
-        <v>0.158575034884208</v>
+        <v>0.158575035</v>
       </c>
       <c r="F5">
         <v>1.01564685536129</v>
@@ -1154,10 +1154,10 @@
         <v>0.0275777466051104</v>
       </c>
       <c r="D6" s="2">
-        <v>0.959784038019155</v>
+        <v>0.959784038</v>
       </c>
       <c r="E6" s="2">
-        <v>0.116524552823414</v>
+        <v>0.116524553</v>
       </c>
       <c r="F6">
         <v>0.821592649807578</v>
@@ -1177,10 +1177,10 @@
         <v>0.0178498353638277</v>
       </c>
       <c r="D7" s="2">
-        <v>0.969431029268869</v>
+        <v>0.969431029</v>
       </c>
       <c r="E7" s="2">
-        <v>0.0942860170783142</v>
+        <v>0.094286017</v>
       </c>
       <c r="F7">
         <v>0.536408332681029</v>
@@ -1200,10 +1200,10 @@
         <v>0.0276982017598</v>
       </c>
       <c r="D8" s="2">
-        <v>0.753018527909132</v>
+        <v>0.753018528</v>
       </c>
       <c r="E8" s="2">
-        <v>0.102221713967372</v>
+        <v>0.102221714</v>
       </c>
       <c r="F8">
         <v>0.280868342057838</v>
@@ -1223,10 +1223,10 @@
         <v>0.0251506598135256</v>
       </c>
       <c r="D9" s="2">
-        <v>0.334670206936775</v>
+        <v>0.334670207</v>
       </c>
       <c r="E9" s="2">
-        <v>0.0500673581664445</v>
+        <v>0.050067358</v>
       </c>
       <c r="F9">
         <v>0.284158244770492</v>
@@ -1246,10 +1246,10 @@
         <v>0.0467241644951738</v>
       </c>
       <c r="D10" s="2">
-        <v>0.191020601887401</v>
+        <v>0.191020602</v>
       </c>
       <c r="E10" s="2">
-        <v>0.0650548210288736</v>
+        <v>0.065054821</v>
       </c>
       <c r="F10">
         <v>0.120809801335442</v>
@@ -1269,10 +1269,10 @@
         <v>0.0584526972115207</v>
       </c>
       <c r="D11" s="2">
-        <v>0.128803685027093</v>
+        <v>0.128803685</v>
       </c>
       <c r="E11" s="2">
-        <v>0.0400771348023738</v>
+        <v>0.040077135</v>
       </c>
       <c r="F11">
         <v>0.121726384511051</v>

</xml_diff>